<commit_message>
Add ORCID Add new columns to LargeDataSetForTexts to account for copyright laws Fixed Bug for reading additonal meta data of texts
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/LargeDataSetForTexts/texts/texts_excel.xlsx
+++ b/tests/testthat/test_data/LargeDataSetForTexts/texts/texts_excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WissMit\Documents\aifeducation\tests\testthat\test_data\LargeDataSetForTexts\texts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA018F5B-B64F-42B9-912F-6A660A92111C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72212FC5-10A8-411E-B8FF-9E59154DC66E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -64,16 +64,51 @@
   </si>
   <si>
     <t>Excel Text C</t>
+  </si>
+  <si>
+    <t>url_license</t>
+  </si>
+  <si>
+    <t>text_license</t>
+  </si>
+  <si>
+    <t>url_source</t>
+  </si>
+  <si>
+    <t>www.source.source.excel_b.xlsx</t>
+  </si>
+  <si>
+    <t>This is a license text for entry b</t>
+  </si>
+  <si>
+    <t>This is a license text for entry a</t>
+  </si>
+  <si>
+    <t>This is a license text for entry c</t>
+  </si>
+  <si>
+    <t>https://test.b.html</t>
+  </si>
+  <si>
+    <t>https://test.a.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,13 +131,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,16 +440,31 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -424,8 +477,17 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -435,8 +497,16 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{A497D3B1-46A6-4307-8A39-61E6B692014F}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{0374B418-5C4A-49E6-A3E2-03AD28874609}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{852736D9-8F6D-4E2F-A87E-F3FBE5D4C679}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>